<commit_message>
updated to UCS.  Animations are in UCS
</commit_message>
<xml_diff>
--- a/MapConfig/map24x24.xlsx
+++ b/MapConfig/map24x24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\OneDrive - MMU\MSc AI\6G7V0011_2324_9F\Week 2\robot js\MapConfig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\Documents\projects\RESTART\MapConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B64691-E9B3-4B33-858C-CBC9CFDE8313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0BF89A-41A7-4C45-ADE1-3E377D5E5785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -339,8 +339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,7 +703,7 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5">
         <v>1</v>
@@ -747,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -948,10 +948,10 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1043,7 +1043,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1132,7 +1132,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1292,7 +1292,7 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T13">
         <v>1</v>
@@ -1410,7 +1410,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1434,7 +1434,7 @@
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15">
         <v>0</v>
@@ -1543,7 +1543,7 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1780,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -1804,7 +1804,7 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R20">
         <v>0</v>

</xml_diff>

<commit_message>
AStar - Test on empty 24x24 map
</commit_message>
<xml_diff>
--- a/MapConfig/map24x24.xlsx
+++ b/MapConfig/map24x24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\Documents\projects\RESTART\MapConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0BF89A-41A7-4C45-ADE1-3E377D5E5785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3781F676-F749-4DFD-B60A-7B1F5F654119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -339,8 +339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,7 +451,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -466,7 +466,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -649,55 +649,55 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -706,13 +706,13 @@
         <v>0</v>
       </c>
       <c r="U5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X5">
         <v>1</v>
@@ -895,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -910,7 +910,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -954,61 +954,61 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9">
         <v>1</v>
@@ -1058,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1191,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1241,52 +1241,52 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -1295,16 +1295,16 @@
         <v>0</v>
       </c>
       <c r="T13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X13">
         <v>1</v>
@@ -1360,7 +1360,7 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R14">
         <v>0</v>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1537,7 +1537,7 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1546,61 +1546,61 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X17">
         <v>1</v>
@@ -1632,7 +1632,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -1656,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -1854,7 +1854,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -1878,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R21">
         <v>0</v>
@@ -1928,7 +1928,7 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -1952,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R22">
         <v>0</v>
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -2026,7 +2026,7 @@
         <v>0</v>
       </c>
       <c r="Q23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R23">
         <v>0</v>

</xml_diff>